<commit_message>
made the imports correct
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bdode\Documents\theorie\Theorie-Project-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ldev1\Documents\programming\Theorie-Project-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0038BDEF-0DBA-4310-92CA-D4C7E7F48FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{583A6152-3FBC-4C43-BB9A-ED7D679B4C89}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>Length</t>
   </si>
@@ -148,13 +147,40 @@
   </si>
   <si>
     <t>C-H heuristic</t>
+  </si>
+  <si>
+    <t>PPCH</t>
+  </si>
+  <si>
+    <t>CPPC</t>
+  </si>
+  <si>
+    <t>HCPHPCPH</t>
+  </si>
+  <si>
+    <t>HCPHPHPH</t>
+  </si>
+  <si>
+    <t>lookadhead 11</t>
+  </si>
+  <si>
+    <t>lookahead 12</t>
+  </si>
+  <si>
+    <t>lookahead 10</t>
+  </si>
+  <si>
+    <t>lookahead 9</t>
+  </si>
+  <si>
+    <t>lookahead 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +208,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -203,12 +235,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,11 +559,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC38666-A880-441F-AAAC-AD36DC983DAE}">
-  <dimension ref="A1:M37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,6 +579,9 @@
     <col min="9" max="9" width="24.5703125" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -692,7 +731,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20</v>
       </c>
@@ -703,7 +742,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>36</v>
       </c>
@@ -714,7 +753,7 @@
         <v>-14</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>50</v>
       </c>
@@ -725,7 +764,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>36</v>
       </c>
@@ -733,7 +772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>36</v>
       </c>
@@ -741,7 +780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>50</v>
       </c>
@@ -749,7 +788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>50</v>
       </c>
@@ -757,16 +796,71 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" t="s">
+        <v>44</v>
+      </c>
+      <c r="L25" t="s">
+        <v>45</v>
+      </c>
+      <c r="M25" t="s">
+        <v>46</v>
+      </c>
+      <c r="N25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C27" t="s">
         <v>32</v>
       </c>
@@ -776,55 +870,411 @@
       <c r="E27" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" t="s">
+        <v>32</v>
+      </c>
+      <c r="L27" t="s">
+        <v>32</v>
+      </c>
+      <c r="M27" t="s">
+        <v>32</v>
+      </c>
+      <c r="N27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>-25</v>
+      </c>
+      <c r="D28">
+        <v>-31</v>
+      </c>
+      <c r="E28">
+        <v>-25</v>
+      </c>
+      <c r="F28">
+        <v>-33</v>
+      </c>
+      <c r="H28">
+        <v>-22</v>
+      </c>
+      <c r="I28">
+        <v>-21</v>
+      </c>
+      <c r="K28">
+        <v>-32</v>
+      </c>
+      <c r="L28">
+        <v>-33</v>
+      </c>
+      <c r="M28">
+        <v>-36</v>
+      </c>
+      <c r="N28">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>-25</v>
+      </c>
+      <c r="D29">
+        <v>-31</v>
+      </c>
+      <c r="E29">
+        <v>-25</v>
+      </c>
+      <c r="F29">
+        <v>-33</v>
+      </c>
+      <c r="H29">
+        <v>-22</v>
+      </c>
+      <c r="I29">
+        <v>-21</v>
+      </c>
+      <c r="K29">
+        <v>-32</v>
+      </c>
+      <c r="L29">
+        <v>-33</v>
+      </c>
+      <c r="M29">
+        <v>-36</v>
+      </c>
+      <c r="N29">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>-25</v>
+      </c>
+      <c r="D30">
+        <v>-31</v>
+      </c>
+      <c r="E30">
+        <v>-27</v>
+      </c>
+      <c r="F30">
+        <v>-32</v>
+      </c>
+      <c r="H30">
+        <v>-22</v>
+      </c>
+      <c r="I30">
+        <v>-21</v>
+      </c>
+      <c r="K30">
+        <v>-32</v>
+      </c>
+      <c r="L30">
+        <v>-32</v>
+      </c>
+      <c r="M30">
+        <v>-36</v>
+      </c>
+      <c r="N30">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>-25</v>
+      </c>
+      <c r="D31">
+        <v>-30</v>
+      </c>
+      <c r="E31">
+        <v>-24</v>
+      </c>
+      <c r="F31">
+        <v>-32</v>
+      </c>
+      <c r="H31">
+        <v>-20</v>
+      </c>
+      <c r="I31">
+        <v>-21</v>
+      </c>
+      <c r="K31">
+        <v>-29</v>
+      </c>
+      <c r="L31">
+        <v>-37</v>
+      </c>
+      <c r="M31">
+        <v>-34</v>
+      </c>
+      <c r="N31">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>-25</v>
+      </c>
+      <c r="D32">
+        <v>-29</v>
+      </c>
+      <c r="E32">
+        <v>-22</v>
+      </c>
+      <c r="F32">
+        <v>-33</v>
+      </c>
+      <c r="H32">
+        <v>-20</v>
+      </c>
+      <c r="I32">
+        <v>-21</v>
+      </c>
+      <c r="K32">
+        <v>-31</v>
+      </c>
+      <c r="L32">
+        <v>-36</v>
+      </c>
+      <c r="M32">
+        <v>-36</v>
+      </c>
+      <c r="N32">
+        <v>-31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>-25</v>
+      </c>
+      <c r="D33">
+        <v>-30</v>
+      </c>
+      <c r="E33">
+        <v>-20</v>
+      </c>
+      <c r="F33">
+        <v>-32</v>
+      </c>
+      <c r="H33">
+        <v>-25</v>
+      </c>
+      <c r="I33">
+        <v>-19</v>
+      </c>
+      <c r="K33">
+        <v>-31</v>
+      </c>
+      <c r="L33">
+        <v>-33</v>
+      </c>
+      <c r="M33">
+        <v>-33</v>
+      </c>
+      <c r="N33">
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>-25</v>
+      </c>
+      <c r="D34">
+        <v>-31</v>
+      </c>
+      <c r="E34">
+        <v>-20</v>
+      </c>
+      <c r="F34">
+        <v>-31</v>
+      </c>
+      <c r="H34">
+        <v>-25</v>
+      </c>
+      <c r="I34">
+        <v>-19</v>
+      </c>
+      <c r="K34">
+        <v>-30</v>
+      </c>
+      <c r="L34">
+        <v>-33</v>
+      </c>
+      <c r="M34">
+        <v>-33</v>
+      </c>
+      <c r="N34">
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>-25</v>
+      </c>
+      <c r="D35">
+        <v>-31</v>
+      </c>
+      <c r="E35">
+        <v>-20</v>
+      </c>
+      <c r="F35">
+        <v>-29</v>
+      </c>
+      <c r="H35">
+        <v>-25</v>
+      </c>
+      <c r="I35">
+        <v>-19</v>
+      </c>
+      <c r="K35">
+        <v>-28</v>
+      </c>
+      <c r="L35">
+        <v>-30</v>
+      </c>
+      <c r="M35">
+        <v>-32</v>
+      </c>
+      <c r="N35">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>-25</v>
+      </c>
+      <c r="D36">
+        <v>-31</v>
+      </c>
+      <c r="E36">
+        <v>-22</v>
+      </c>
+      <c r="F36">
+        <v>-29</v>
+      </c>
+      <c r="H36">
+        <v>-25</v>
+      </c>
+      <c r="I36">
+        <v>-19</v>
+      </c>
+      <c r="K36">
+        <v>-28</v>
+      </c>
+      <c r="L36">
+        <v>-33</v>
+      </c>
+      <c r="M36">
+        <v>-33</v>
+      </c>
+      <c r="N36">
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>31</v>
+      </c>
+      <c r="C37">
+        <v>-25</v>
+      </c>
+      <c r="D37">
+        <v>-31</v>
+      </c>
+      <c r="E37">
+        <v>-22</v>
+      </c>
+      <c r="F37">
+        <v>-29</v>
+      </c>
+      <c r="H37">
+        <v>-25</v>
+      </c>
+      <c r="I37">
+        <v>-19</v>
+      </c>
+      <c r="K37">
+        <v>-28</v>
+      </c>
+      <c r="L37">
+        <v>-33</v>
+      </c>
+      <c r="M37">
+        <v>-33</v>
+      </c>
+      <c r="N37">
+        <v>-33</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" s="5">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>-25</v>
+      </c>
+      <c r="D38">
+        <v>-31</v>
+      </c>
+      <c r="E38">
+        <v>-25</v>
+      </c>
+      <c r="F38">
+        <v>-31</v>
+      </c>
+      <c r="H38">
+        <v>-24</v>
+      </c>
+      <c r="I38">
+        <v>-18</v>
+      </c>
+      <c r="K38">
+        <v>-28</v>
+      </c>
+      <c r="L38">
+        <v>-33</v>
+      </c>
+      <c r="M38">
+        <v>-33</v>
+      </c>
+      <c r="N38">
+        <v>-33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>